<commit_message>
some tweet with final excel for SFN
</commit_message>
<xml_diff>
--- a/Final sheet.xlsx
+++ b/Final sheet.xlsx
@@ -203,10 +203,10 @@
     <t>Dbl HET</t>
   </si>
   <si>
-    <t>E1ko; E2 HET</t>
+    <t>E1 HET; E2 cKO</t>
   </si>
   <si>
-    <t>E1 HET;E2cKO</t>
+    <t>E1 ko; E2 HET</t>
   </si>
 </sst>
 </file>
@@ -629,7 +629,7 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="49" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C49" s="1">
         <v>1.3591981132075472</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="50" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C50" s="1">
         <v>0.8322851153039833</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="51" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C51" s="1">
         <v>0.47672955974842757</v>
@@ -2254,7 +2254,7 @@
     </row>
     <row r="52" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C52" s="1">
         <v>0.82704402515723263</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="53" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C53" s="1">
         <v>0.88003144654088039</v>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="54" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C54" s="1">
         <v>0.89203354297693904</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="55" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C55" s="1">
         <v>1.0257861635220125</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="56" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C56" s="1">
         <v>1.040503144654088</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="57" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C57" s="1">
         <v>0.97924528301886771</v>
@@ -2446,7 +2446,7 @@
     </row>
     <row r="58" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C58" s="1">
         <v>0.7278616352201257</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="59" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C59" s="1">
         <v>1.1591194968553458</v>

</xml_diff>

<commit_message>
Second changes at the final excel sheet for SFN
</commit_message>
<xml_diff>
--- a/Final sheet.xlsx
+++ b/Final sheet.xlsx
@@ -203,10 +203,10 @@
     <t>Dbl HET</t>
   </si>
   <si>
-    <t>E1 HET; E2 cKO</t>
+    <t>E1ko; E2 HET</t>
   </si>
   <si>
-    <t>E1 ko; E2 HET</t>
+    <t>E1 HET; E2cKO</t>
   </si>
 </sst>
 </file>
@@ -629,7 +629,7 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="49" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C49" s="1">
         <v>1.3591981132075472</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="50" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C50" s="1">
         <v>0.8322851153039833</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="51" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C51" s="1">
         <v>0.47672955974842757</v>
@@ -2254,7 +2254,7 @@
     </row>
     <row r="52" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C52" s="1">
         <v>0.82704402515723263</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="53" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C53" s="1">
         <v>0.88003144654088039</v>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="54" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C54" s="1">
         <v>0.89203354297693904</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="55" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C55" s="1">
         <v>1.0257861635220125</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="56" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C56" s="1">
         <v>1.040503144654088</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="57" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C57" s="1">
         <v>0.97924528301886771</v>
@@ -2446,7 +2446,7 @@
     </row>
     <row r="58" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C58" s="1">
         <v>0.7278616352201257</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="59" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C59" s="1">
         <v>1.1591194968553458</v>

</xml_diff>